<commit_message>
admin page plus data
</commit_message>
<xml_diff>
--- a/details.xlsx
+++ b/details.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,23 +544,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mahesh Krishna Reddy</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>sai</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Vanga</t>
+          <t>j</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>8134182519</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>m_vanga@uncg.edu</t>
+          <t>saipjaligama@gmail.com</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -569,26 +573,68 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1999-10-06</t>
+          <t>2023-10-25</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1002 Bitting St Greensboro</t>
+          <t>5035 s east end S2402
+s2402</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>ILLINOIS</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Preferred non tobacco</t>
+          <t>Preferred Plus Non Tobacco</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>200000</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>maximum</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>ltc_rider</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>2%</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Preferred Tobacco</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>10-Year</t>
         </is>
       </c>
     </row>
@@ -598,27 +644,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>mahesh</t>
+          <t>Sai</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>krishna</t>
+          <t>p</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>reddy</t>
+          <t>p</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>9740072090</t>
+          <t>8155933548</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>maheshkrishnareddy@gmail.com</t>
+          <t>saijaligama@hotmail.com</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -627,84 +673,71 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1999-10-06</t>
+          <t>2023-10-04</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1002 bitting st</t>
+          <t>13804 Summit Commons BLvd apt I</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>xyz</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>mahesh</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>krishna</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>reddy</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>9740072090</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>maheshkrishy@gmail.com</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>24</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2023-09-20</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>qqqqq</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>qqqqqq</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
           <t>Preferred Plus Non Tobacco</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>22222</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>maximum</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>ltc_rider</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>2%</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Preferred Tobacco</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>10-Year</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updates shceduler, home and download and by id
</commit_message>
<xml_diff>
--- a/details.xlsx
+++ b/details.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,26 +540,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ais</t>
+          <t>nejnen</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>sjnvjdn</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ee</t>
+          <t>iejejiei</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>32sa</t>
+          <t>93837897</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -573,21 +573,21 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>2020-02-02</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>3223</t>
+          <t>nwjnwjn</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>il3</t>
+          <t>il</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -597,7 +597,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2322323</t>
+          <t>89999</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -622,7 +622,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>2323</t>
+          <t>9999</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -640,210 +640,14 @@
           <t>10-Year</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>sai</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>j</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>i</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>saipjaligama@gmail.com</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>22</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2023-02-07</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>2i</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>ll33</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Preferred Plus Non Tobacco</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>monthly</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>maximum</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>ltc_rider</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>0000</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>2%</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Preferred Tobacco</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>10-Year</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ja</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ji</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>ii8</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>888</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>saijaligama@hotmail.com</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>male</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>23</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2023-11-07</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>00000</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>hj23</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Preferred Plus Non Tobacco</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>23323</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>level</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>monthly</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>maximum</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>ltc_rider</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>23232</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>2%</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Preferred Tobacco</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>10-Year</t>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>2 Years</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added shceduler to chatbot and changes
</commit_message>
<xml_diff>
--- a/details.xlsx
+++ b/details.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,26 +540,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>nejnen</t>
+          <t>Jaligama</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sjnvjdn</t>
+          <t>Prabhu</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>iejejiei</t>
+          <t>Jaligama</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>93837897</t>
+          <t>8155933548</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -572,22 +572,17 @@
           <t>male</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>88</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2020-02-02</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>nwjnwjn</t>
+          <t>5035 s east end S2402
+s2402</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>il</t>
+          <t>ILLINOIS</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -595,11 +590,7 @@
           <t>Preferred Plus Non Tobacco</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>89999</t>
-        </is>
-      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
           <t>level</t>
@@ -620,11 +611,7 @@
           <t>ltc_rider</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>9999</t>
-        </is>
-      </c>
+      <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr">
         <is>
           <t>2%</t>
@@ -640,12 +627,12 @@
           <t>10-Year</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>2 Years</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>None</t>
         </is>

</xml_diff>